<commit_message>
sku list for making test cases
</commit_message>
<xml_diff>
--- a/ShopCart/ProductIDList.xlsx
+++ b/ShopCart/ProductIDList.xlsx
@@ -1024,9 +1024,6 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -1034,6 +1031,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -26302,7 +26302,8 @@
   <dimension ref="A1:K112"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="26.42578125" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -26311,8 +26312,8 @@
     <col min="2" max="2" width="16.85546875" style="4" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7.7109375" style="4" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="1.5703125" style="8" customWidth="1"/>
-    <col min="6" max="6" width="19.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="1.5703125" style="7" customWidth="1"/>
     <col min="7" max="7" width="7.42578125" style="4" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="20.7109375" style="4" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="5.85546875" style="4" bestFit="1" customWidth="1"/>
@@ -26322,34 +26323,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="9" t="s">
         <v>309</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="8" t="s">
         <v>300</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="8" t="s">
         <v>307</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="8" t="s">
         <v>302</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="E1" s="10" t="s">
         <v>308</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" s="6" t="s">
         <v>301</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="H1" s="6" t="s">
         <v>303</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="I1" s="6" t="s">
         <v>304</v>
       </c>
-      <c r="J1" s="7" t="s">
+      <c r="J1" s="6" t="s">
         <v>305</v>
       </c>
-      <c r="K1" s="7" t="s">
+      <c r="K1" s="6" t="s">
         <v>306</v>
       </c>
     </row>
@@ -26366,7 +26367,7 @@
       <c r="D2" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="E2" s="5" t="s">
         <v>193</v>
       </c>
       <c r="G2" s="5" t="b">
@@ -26398,7 +26399,7 @@
       <c r="D3" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="E3" s="5" t="s">
         <v>193</v>
       </c>
       <c r="G3" s="5" t="b">
@@ -26430,7 +26431,7 @@
       <c r="D4" s="5" t="s">
         <v>161</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="E4" s="5" t="s">
         <v>160</v>
       </c>
       <c r="G4" s="5" t="b">
@@ -26462,7 +26463,7 @@
       <c r="D5" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="E5" s="5" t="s">
         <v>225</v>
       </c>
       <c r="G5" s="5" t="b">
@@ -26494,7 +26495,7 @@
       <c r="D6" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="F6" s="5" t="s">
+      <c r="E6" s="5" t="s">
         <v>225</v>
       </c>
       <c r="G6" s="5" t="b">
@@ -26526,7 +26527,7 @@
       <c r="D7" s="5" t="s">
         <v>224</v>
       </c>
-      <c r="F7" s="5" t="s">
+      <c r="E7" s="5" t="s">
         <v>223</v>
       </c>
       <c r="G7" s="5" t="b">
@@ -26558,7 +26559,7 @@
       <c r="D8" s="5" t="s">
         <v>224</v>
       </c>
-      <c r="F8" s="5" t="s">
+      <c r="E8" s="5" t="s">
         <v>223</v>
       </c>
       <c r="G8" s="5" t="b">
@@ -26590,7 +26591,7 @@
       <c r="D9" s="5" t="s">
         <v>263</v>
       </c>
-      <c r="F9" s="5" t="s">
+      <c r="E9" s="5" t="s">
         <v>262</v>
       </c>
       <c r="G9" s="5" t="b">
@@ -26622,7 +26623,7 @@
       <c r="D10" s="5" t="s">
         <v>263</v>
       </c>
-      <c r="F10" s="5" t="s">
+      <c r="E10" s="5" t="s">
         <v>262</v>
       </c>
       <c r="G10" s="5" t="b">
@@ -26654,7 +26655,7 @@
       <c r="D11" s="5" t="s">
         <v>261</v>
       </c>
-      <c r="F11" s="5" t="s">
+      <c r="E11" s="5" t="s">
         <v>260</v>
       </c>
       <c r="G11" s="5" t="b">
@@ -26686,7 +26687,7 @@
       <c r="D12" s="5" t="s">
         <v>261</v>
       </c>
-      <c r="F12" s="5" t="s">
+      <c r="E12" s="5" t="s">
         <v>260</v>
       </c>
       <c r="G12" s="5" t="b">
@@ -26718,7 +26719,7 @@
       <c r="D13" s="5" t="s">
         <v>130</v>
       </c>
-      <c r="F13" s="5" t="s">
+      <c r="E13" s="5" t="s">
         <v>235</v>
       </c>
       <c r="G13" s="5" t="b">
@@ -26750,7 +26751,7 @@
       <c r="D14" s="5" t="s">
         <v>130</v>
       </c>
-      <c r="F14" s="5" t="s">
+      <c r="E14" s="5" t="s">
         <v>235</v>
       </c>
       <c r="G14" s="5" t="b">
@@ -26782,7 +26783,7 @@
       <c r="D15" s="5" t="s">
         <v>234</v>
       </c>
-      <c r="F15" s="5" t="s">
+      <c r="E15" s="5" t="s">
         <v>233</v>
       </c>
       <c r="G15" s="5" t="b">
@@ -26814,7 +26815,7 @@
       <c r="D16" s="5" t="s">
         <v>234</v>
       </c>
-      <c r="F16" s="5" t="s">
+      <c r="E16" s="5" t="s">
         <v>233</v>
       </c>
       <c r="G16" s="5" t="b">
@@ -26846,7 +26847,7 @@
       <c r="D17" s="5" t="s">
         <v>237</v>
       </c>
-      <c r="F17" s="5" t="s">
+      <c r="E17" s="5" t="s">
         <v>236</v>
       </c>
       <c r="G17" s="5" t="b">
@@ -26878,7 +26879,7 @@
       <c r="D18" s="5" t="s">
         <v>237</v>
       </c>
-      <c r="F18" s="5" t="s">
+      <c r="E18" s="5" t="s">
         <v>236</v>
       </c>
       <c r="G18" s="5" t="b">
@@ -26910,7 +26911,7 @@
       <c r="D19" s="5" t="s">
         <v>190</v>
       </c>
-      <c r="F19" s="5" t="s">
+      <c r="E19" s="5" t="s">
         <v>189</v>
       </c>
       <c r="G19" s="5" t="b">
@@ -26942,7 +26943,7 @@
       <c r="D20" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="F20" s="5" t="s">
+      <c r="E20" s="5" t="s">
         <v>193</v>
       </c>
       <c r="G20" s="5" t="b">
@@ -26974,7 +26975,7 @@
       <c r="D21" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="F21" s="5" t="s">
+      <c r="E21" s="5" t="s">
         <v>193</v>
       </c>
       <c r="G21" s="5" t="b">
@@ -27006,7 +27007,7 @@
       <c r="D22" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="F22" s="5" t="s">
+      <c r="E22" s="5" t="s">
         <v>195</v>
       </c>
       <c r="G22" s="5" t="b">
@@ -27038,7 +27039,7 @@
       <c r="D23" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="F23" s="5" t="s">
+      <c r="E23" s="5" t="s">
         <v>251</v>
       </c>
       <c r="G23" s="5" t="b">
@@ -27070,7 +27071,7 @@
       <c r="D24" s="5" t="s">
         <v>227</v>
       </c>
-      <c r="F24" s="5" t="s">
+      <c r="E24" s="5" t="s">
         <v>226</v>
       </c>
       <c r="G24" s="5" t="b">
@@ -27102,7 +27103,7 @@
       <c r="D25" s="5" t="s">
         <v>247</v>
       </c>
-      <c r="F25" s="5" t="s">
+      <c r="E25" s="5" t="s">
         <v>246</v>
       </c>
       <c r="G25" s="5" t="b">
@@ -27134,7 +27135,7 @@
       <c r="D26" s="5" t="s">
         <v>247</v>
       </c>
-      <c r="F26" s="5" t="s">
+      <c r="E26" s="5" t="s">
         <v>246</v>
       </c>
       <c r="G26" s="5" t="b">
@@ -27166,7 +27167,7 @@
       <c r="D27" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="F27" s="5" t="s">
+      <c r="E27" s="5" t="s">
         <v>248</v>
       </c>
       <c r="G27" s="5" t="b">
@@ -27198,7 +27199,7 @@
       <c r="D28" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="F28" s="5" t="s">
+      <c r="E28" s="5" t="s">
         <v>248</v>
       </c>
       <c r="G28" s="5" t="b">
@@ -27230,7 +27231,7 @@
       <c r="D29" s="5" t="s">
         <v>250</v>
       </c>
-      <c r="F29" s="5" t="s">
+      <c r="E29" s="5" t="s">
         <v>249</v>
       </c>
       <c r="G29" s="5" t="b">
@@ -27262,7 +27263,7 @@
       <c r="D30" s="5" t="s">
         <v>250</v>
       </c>
-      <c r="F30" s="5" t="s">
+      <c r="E30" s="5" t="s">
         <v>249</v>
       </c>
       <c r="G30" s="5" t="b">
@@ -27294,7 +27295,7 @@
       <c r="D31" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="F31" s="5" t="s">
+      <c r="E31" s="5" t="s">
         <v>251</v>
       </c>
       <c r="G31" s="5" t="b">
@@ -27326,7 +27327,7 @@
       <c r="D32" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="F32" s="5" t="s">
+      <c r="E32" s="5" t="s">
         <v>193</v>
       </c>
       <c r="G32" s="5" t="b">
@@ -27358,7 +27359,7 @@
       <c r="D33" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="F33" s="5" t="s">
+      <c r="E33" s="5" t="s">
         <v>157</v>
       </c>
       <c r="G33" s="5" t="b">
@@ -27390,7 +27391,7 @@
       <c r="D34" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="F34" s="5" t="s">
+      <c r="E34" s="5" t="s">
         <v>137</v>
       </c>
       <c r="G34" s="5" t="b">
@@ -27422,7 +27423,7 @@
       <c r="D35" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="F35" s="5" t="s">
+      <c r="E35" s="5" t="s">
         <v>149</v>
       </c>
       <c r="G35" s="5" t="b">
@@ -27454,7 +27455,7 @@
       <c r="D36" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="F36" s="5" t="s">
+      <c r="E36" s="5" t="s">
         <v>154</v>
       </c>
       <c r="G36" s="5" t="b">
@@ -27486,7 +27487,7 @@
       <c r="D37" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="F37" s="5" t="s">
+      <c r="E37" s="5" t="s">
         <v>142</v>
       </c>
       <c r="G37" s="5" t="b">
@@ -27518,7 +27519,7 @@
       <c r="D38" s="5" t="s">
         <v>231</v>
       </c>
-      <c r="F38" s="5" t="s">
+      <c r="E38" s="5" t="s">
         <v>230</v>
       </c>
       <c r="G38" s="5" t="b">
@@ -27550,7 +27551,7 @@
       <c r="D39" s="5" t="s">
         <v>229</v>
       </c>
-      <c r="F39" s="5" t="s">
+      <c r="E39" s="5" t="s">
         <v>228</v>
       </c>
       <c r="G39" s="5" t="b">
@@ -27582,7 +27583,7 @@
       <c r="D40" s="5" t="s">
         <v>141</v>
       </c>
-      <c r="F40" s="5" t="s">
+      <c r="E40" s="5" t="s">
         <v>232</v>
       </c>
       <c r="G40" s="5" t="b">
@@ -27614,7 +27615,7 @@
       <c r="D41" s="5" t="s">
         <v>245</v>
       </c>
-      <c r="F41" s="5" t="s">
+      <c r="E41" s="5" t="s">
         <v>244</v>
       </c>
       <c r="G41" s="5" t="b">
@@ -27646,7 +27647,7 @@
       <c r="D42" s="5" t="s">
         <v>175</v>
       </c>
-      <c r="F42" s="5" t="s">
+      <c r="E42" s="5" t="s">
         <v>174</v>
       </c>
       <c r="G42" s="5" t="b">
@@ -27678,7 +27679,7 @@
       <c r="D43" s="5" t="s">
         <v>167</v>
       </c>
-      <c r="F43" s="5" t="s">
+      <c r="E43" s="5" t="s">
         <v>166</v>
       </c>
       <c r="G43" s="5" t="b">
@@ -27710,7 +27711,7 @@
       <c r="D44" s="5" t="s">
         <v>169</v>
       </c>
-      <c r="F44" s="5" t="s">
+      <c r="E44" s="5" t="s">
         <v>168</v>
       </c>
       <c r="G44" s="5" t="b">
@@ -27742,7 +27743,7 @@
       <c r="D45" s="5" t="s">
         <v>171</v>
       </c>
-      <c r="F45" s="5" t="s">
+      <c r="E45" s="5" t="s">
         <v>170</v>
       </c>
       <c r="G45" s="5" t="b">
@@ -27774,7 +27775,7 @@
       <c r="D46" s="5" t="s">
         <v>173</v>
       </c>
-      <c r="F46" s="5" t="s">
+      <c r="E46" s="5" t="s">
         <v>172</v>
       </c>
       <c r="G46" s="5" t="b">
@@ -27806,7 +27807,7 @@
       <c r="D47" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="F47" s="5" t="s">
+      <c r="E47" s="5" t="s">
         <v>269</v>
       </c>
       <c r="G47" s="5" t="b">
@@ -27838,7 +27839,7 @@
       <c r="D48" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="F48" s="5" t="s">
+      <c r="E48" s="5" t="s">
         <v>269</v>
       </c>
       <c r="G48" s="5" t="b">
@@ -27870,7 +27871,7 @@
       <c r="D49" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="F49" s="5" t="s">
+      <c r="E49" s="5" t="s">
         <v>221</v>
       </c>
       <c r="G49" s="5" t="b">
@@ -27902,7 +27903,7 @@
       <c r="D50" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="F50" s="5" t="s">
+      <c r="E50" s="5" t="s">
         <v>221</v>
       </c>
       <c r="G50" s="5" t="b">
@@ -27934,7 +27935,7 @@
       <c r="D51" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="F51" s="5" t="s">
+      <c r="E51" s="5" t="s">
         <v>165</v>
       </c>
       <c r="G51" s="5" t="b">
@@ -27966,7 +27967,7 @@
       <c r="D52" s="5" t="s">
         <v>243</v>
       </c>
-      <c r="F52" s="5" t="s">
+      <c r="E52" s="5" t="s">
         <v>243</v>
       </c>
       <c r="G52" s="5" t="b">
@@ -27998,7 +27999,7 @@
       <c r="D53" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="F53" s="5" t="s">
+      <c r="E53" s="5" t="s">
         <v>252</v>
       </c>
       <c r="G53" s="5" t="b">
@@ -28030,7 +28031,7 @@
       <c r="D54" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="F54" s="5" t="s">
+      <c r="E54" s="5" t="s">
         <v>176</v>
       </c>
       <c r="G54" s="5" t="b">
@@ -28062,7 +28063,7 @@
       <c r="D55" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F55" s="5" t="s">
+      <c r="E55" s="5" t="s">
         <v>178</v>
       </c>
       <c r="G55" s="5" t="b">
@@ -28094,7 +28095,7 @@
       <c r="D56" s="5" t="s">
         <v>182</v>
       </c>
-      <c r="F56" s="5" t="s">
+      <c r="E56" s="5" t="s">
         <v>180</v>
       </c>
       <c r="G56" s="5" t="b">
@@ -28126,7 +28127,7 @@
       <c r="D57" s="5" t="s">
         <v>185</v>
       </c>
-      <c r="F57" s="5" t="s">
+      <c r="E57" s="5" t="s">
         <v>183</v>
       </c>
       <c r="G57" s="5" t="b">
@@ -28158,7 +28159,7 @@
       <c r="D58" s="5" t="s">
         <v>188</v>
       </c>
-      <c r="F58" s="5" t="s">
+      <c r="E58" s="5" t="s">
         <v>186</v>
       </c>
       <c r="G58" s="5" t="b">
@@ -28190,7 +28191,7 @@
       <c r="D59" s="5" t="s">
         <v>206</v>
       </c>
-      <c r="F59" s="5" t="s">
+      <c r="E59" s="5" t="s">
         <v>204</v>
       </c>
       <c r="G59" s="5" t="b">
@@ -28222,7 +28223,7 @@
       <c r="D60" s="5" t="s">
         <v>203</v>
       </c>
-      <c r="F60" s="5" t="s">
+      <c r="E60" s="5" t="s">
         <v>201</v>
       </c>
       <c r="G60" s="5" t="b">
@@ -28254,7 +28255,7 @@
       <c r="D61" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="F61" s="5" t="s">
+      <c r="E61" s="5" t="s">
         <v>207</v>
       </c>
       <c r="G61" s="5" t="b">
@@ -28286,7 +28287,7 @@
       <c r="D62" s="5" t="s">
         <v>213</v>
       </c>
-      <c r="F62" s="5" t="s">
+      <c r="E62" s="5" t="s">
         <v>211</v>
       </c>
       <c r="G62" s="5" t="b">
@@ -28318,7 +28319,7 @@
       <c r="D63" s="5" t="s">
         <v>217</v>
       </c>
-      <c r="F63" s="5" t="s">
+      <c r="E63" s="5" t="s">
         <v>215</v>
       </c>
       <c r="G63" s="5" t="b">
@@ -28350,7 +28351,7 @@
       <c r="D64" s="5" t="s">
         <v>255</v>
       </c>
-      <c r="F64" s="5" t="s">
+      <c r="E64" s="5" t="s">
         <v>253</v>
       </c>
       <c r="G64" s="5" t="b">
@@ -28382,7 +28383,7 @@
       <c r="D65" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="F65" s="5" t="s">
+      <c r="E65" s="5" t="s">
         <v>222</v>
       </c>
       <c r="G65" s="5" t="b">
@@ -28414,7 +28415,7 @@
       <c r="D66" s="5" t="s">
         <v>199</v>
       </c>
-      <c r="F66" s="5" t="s">
+      <c r="E66" s="5" t="s">
         <v>198</v>
       </c>
       <c r="G66" s="5" t="b">
@@ -28446,7 +28447,7 @@
       <c r="D67" s="5" t="s">
         <v>257</v>
       </c>
-      <c r="F67" s="5" t="s">
+      <c r="E67" s="5" t="s">
         <v>256</v>
       </c>
       <c r="G67" s="5" t="b">
@@ -28478,7 +28479,7 @@
       <c r="D68" s="5" t="s">
         <v>164</v>
       </c>
-      <c r="F68" s="5" t="s">
+      <c r="E68" s="5" t="s">
         <v>163</v>
       </c>
       <c r="G68" s="5" t="b">
@@ -28510,7 +28511,7 @@
       <c r="D69" s="5" t="s">
         <v>146</v>
       </c>
-      <c r="F69" s="5" t="s">
+      <c r="E69" s="5" t="s">
         <v>145</v>
       </c>
       <c r="G69" s="5" t="b">
@@ -28542,7 +28543,7 @@
       <c r="D70" s="5" t="s">
         <v>153</v>
       </c>
-      <c r="F70" s="5" t="s">
+      <c r="E70" s="5" t="s">
         <v>152</v>
       </c>
       <c r="G70" s="5" t="b">
@@ -28574,7 +28575,7 @@
       <c r="D71" s="5" t="s">
         <v>148</v>
       </c>
-      <c r="F71" s="5" t="s">
+      <c r="E71" s="5" t="s">
         <v>147</v>
       </c>
       <c r="G71" s="5" t="b">
@@ -28606,7 +28607,7 @@
       <c r="D72" s="5" t="s">
         <v>153</v>
       </c>
-      <c r="F72" s="5" t="s">
+      <c r="E72" s="5" t="s">
         <v>152</v>
       </c>
       <c r="G72" s="5" t="b">
@@ -28638,7 +28639,7 @@
       <c r="D73" s="5" t="s">
         <v>164</v>
       </c>
-      <c r="F73" s="5" t="s">
+      <c r="E73" s="5" t="s">
         <v>163</v>
       </c>
       <c r="G73" s="5" t="b">
@@ -28670,7 +28671,7 @@
       <c r="D74" s="5" t="s">
         <v>146</v>
       </c>
-      <c r="F74" s="5" t="s">
+      <c r="E74" s="5" t="s">
         <v>145</v>
       </c>
       <c r="G74" s="5" t="b">
@@ -28702,7 +28703,7 @@
       <c r="D75" s="5" t="s">
         <v>148</v>
       </c>
-      <c r="F75" s="5" t="s">
+      <c r="E75" s="5" t="s">
         <v>147</v>
       </c>
       <c r="G75" s="5" t="b">
@@ -28734,7 +28735,7 @@
       <c r="D76" s="5" t="s">
         <v>265</v>
       </c>
-      <c r="F76" s="5" t="s">
+      <c r="E76" s="5" t="s">
         <v>264</v>
       </c>
       <c r="G76" s="5" t="b">
@@ -28766,7 +28767,7 @@
       <c r="D77" s="5" t="s">
         <v>141</v>
       </c>
-      <c r="F77" s="5" t="s">
+      <c r="E77" s="5" t="s">
         <v>140</v>
       </c>
       <c r="G77" s="5" t="b">
@@ -28798,7 +28799,7 @@
       <c r="D78" s="5" t="s">
         <v>141</v>
       </c>
-      <c r="F78" s="5" t="s">
+      <c r="E78" s="5" t="s">
         <v>140</v>
       </c>
       <c r="G78" s="5" t="b">
@@ -28830,7 +28831,7 @@
       <c r="D79" s="5" t="s">
         <v>265</v>
       </c>
-      <c r="F79" s="5" t="s">
+      <c r="E79" s="5" t="s">
         <v>264</v>
       </c>
       <c r="G79" s="5" t="b">
@@ -28862,7 +28863,7 @@
       <c r="D80" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="F80" s="5" t="s">
+      <c r="E80" s="5" t="s">
         <v>162</v>
       </c>
       <c r="G80" s="5" t="b">
@@ -28894,7 +28895,7 @@
       <c r="D81" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="F81" s="5" t="s">
+      <c r="E81" s="5" t="s">
         <v>162</v>
       </c>
       <c r="G81" s="5" t="b">
@@ -28926,7 +28927,7 @@
       <c r="D82" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="F82" s="5" t="s">
+      <c r="E82" s="5" t="s">
         <v>194</v>
       </c>
       <c r="G82" s="5" t="b">
@@ -28958,7 +28959,7 @@
       <c r="D83" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="F83" s="5" t="s">
+      <c r="E83" s="5" t="s">
         <v>194</v>
       </c>
       <c r="G83" s="5" t="b">
@@ -28990,7 +28991,7 @@
       <c r="D84" s="5" t="s">
         <v>197</v>
       </c>
-      <c r="F84" s="5" t="s">
+      <c r="E84" s="5" t="s">
         <v>196</v>
       </c>
       <c r="G84" s="5" t="b">
@@ -29022,7 +29023,7 @@
       <c r="D85" s="5" t="s">
         <v>241</v>
       </c>
-      <c r="F85" s="5" t="s">
+      <c r="E85" s="5" t="s">
         <v>61</v>
       </c>
       <c r="G85" s="5" t="b">
@@ -29054,7 +29055,7 @@
       <c r="D86" s="5" t="s">
         <v>241</v>
       </c>
-      <c r="F86" s="5" t="s">
+      <c r="E86" s="5" t="s">
         <v>61</v>
       </c>
       <c r="G86" s="5" t="b">
@@ -29086,7 +29087,7 @@
       <c r="D87" s="5" t="s">
         <v>268</v>
       </c>
-      <c r="F87" s="5" t="s">
+      <c r="E87" s="5" t="s">
         <v>268</v>
       </c>
       <c r="G87" s="5" t="b">
@@ -29118,7 +29119,7 @@
       <c r="D88" s="5" t="s">
         <v>268</v>
       </c>
-      <c r="F88" s="5" t="s">
+      <c r="E88" s="5" t="s">
         <v>268</v>
       </c>
       <c r="G88" s="5" t="b">
@@ -29150,7 +29151,7 @@
       <c r="D89" s="5" t="s">
         <v>268</v>
       </c>
-      <c r="F89" s="5" t="s">
+      <c r="E89" s="5" t="s">
         <v>268</v>
       </c>
       <c r="G89" s="5" t="b">
@@ -29182,7 +29183,7 @@
       <c r="D90" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="F90" s="5" t="s">
+      <c r="E90" s="5" t="s">
         <v>219</v>
       </c>
       <c r="G90" s="5" t="b">
@@ -29214,7 +29215,7 @@
       <c r="D91" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="F91" s="5" t="s">
+      <c r="E91" s="5" t="s">
         <v>191</v>
       </c>
       <c r="G91" s="5" t="b">
@@ -29246,7 +29247,7 @@
       <c r="D92" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="F92" s="5" t="s">
+      <c r="E92" s="5" t="s">
         <v>259</v>
       </c>
       <c r="G92" s="5" t="b">
@@ -29278,7 +29279,7 @@
       <c r="D93" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="F93" s="5" t="s">
+      <c r="E93" s="5" t="s">
         <v>192</v>
       </c>
       <c r="G93" s="5" t="b">
@@ -29310,7 +29311,7 @@
       <c r="D94" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="F94" s="5" t="s">
+      <c r="E94" s="5" t="s">
         <v>192</v>
       </c>
       <c r="G94" s="5" t="b">
@@ -29342,7 +29343,7 @@
       <c r="D95" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="F95" s="5" t="s">
+      <c r="E95" s="5" t="s">
         <v>219</v>
       </c>
       <c r="G95" s="5" t="b">
@@ -29374,7 +29375,7 @@
       <c r="D96" s="5" t="s">
         <v>267</v>
       </c>
-      <c r="F96" s="5" t="s">
+      <c r="E96" s="5" t="s">
         <v>266</v>
       </c>
       <c r="G96" s="5" t="b">
@@ -29406,7 +29407,7 @@
       <c r="D97" s="5" t="s">
         <v>267</v>
       </c>
-      <c r="F97" s="5" t="s">
+      <c r="E97" s="5" t="s">
         <v>266</v>
       </c>
       <c r="G97" s="5" t="b">
@@ -29438,7 +29439,7 @@
       <c r="D98" s="5" t="s">
         <v>239</v>
       </c>
-      <c r="F98" s="5" t="s">
+      <c r="E98" s="5" t="s">
         <v>238</v>
       </c>
       <c r="G98" s="5" t="b">
@@ -29470,7 +29471,7 @@
       <c r="D99" s="5" t="s">
         <v>239</v>
       </c>
-      <c r="F99" s="5" t="s">
+      <c r="E99" s="5" t="s">
         <v>238</v>
       </c>
       <c r="G99" s="5" t="b">
@@ -29502,7 +29503,7 @@
       <c r="D100" s="5" t="s">
         <v>240</v>
       </c>
-      <c r="F100" s="5" t="s">
+      <c r="E100" s="5" t="s">
         <v>42</v>
       </c>
       <c r="G100" s="5" t="b">
@@ -29534,7 +29535,7 @@
       <c r="D101" s="5" t="s">
         <v>240</v>
       </c>
-      <c r="F101" s="5" t="s">
+      <c r="E101" s="5" t="s">
         <v>42</v>
       </c>
       <c r="G101" s="5" t="b">
@@ -29566,7 +29567,7 @@
       <c r="D102" s="5" t="s">
         <v>242</v>
       </c>
-      <c r="F102" s="5" t="s">
+      <c r="E102" s="5" t="s">
         <v>39</v>
       </c>
       <c r="G102" s="5" t="b">
@@ -29598,7 +29599,7 @@
       <c r="D103" s="5" t="s">
         <v>242</v>
       </c>
-      <c r="F103" s="5" t="s">
+      <c r="E103" s="5" t="s">
         <v>39</v>
       </c>
       <c r="G103" s="5" t="b">
@@ -29630,7 +29631,7 @@
       <c r="D104" s="5" t="s">
         <v>268</v>
       </c>
-      <c r="F104" s="5" t="s">
+      <c r="E104" s="5" t="s">
         <v>268</v>
       </c>
       <c r="G104" s="5" t="b">
@@ -29662,7 +29663,7 @@
       <c r="D105" s="5" t="s">
         <v>268</v>
       </c>
-      <c r="F105" s="5" t="s">
+      <c r="E105" s="5" t="s">
         <v>268</v>
       </c>
       <c r="G105" s="5" t="b">
@@ -29694,7 +29695,7 @@
       <c r="D106" s="5" t="s">
         <v>268</v>
       </c>
-      <c r="F106" s="5" t="s">
+      <c r="E106" s="5" t="s">
         <v>268</v>
       </c>
       <c r="G106" s="5" t="b">
@@ -29726,7 +29727,7 @@
       <c r="D107" s="5" t="s">
         <v>268</v>
       </c>
-      <c r="F107" s="5" t="s">
+      <c r="E107" s="5" t="s">
         <v>268</v>
       </c>
       <c r="G107" s="5" t="b">
@@ -29758,7 +29759,7 @@
       <c r="D108" s="5" t="s">
         <v>268</v>
       </c>
-      <c r="F108" s="5" t="s">
+      <c r="E108" s="5" t="s">
         <v>268</v>
       </c>
       <c r="G108" s="5" t="b">
@@ -29790,7 +29791,7 @@
       <c r="D109" s="5" t="s">
         <v>268</v>
       </c>
-      <c r="F109" s="5" t="s">
+      <c r="E109" s="5" t="s">
         <v>268</v>
       </c>
       <c r="G109" s="5" t="b">
@@ -29822,7 +29823,7 @@
       <c r="D110" s="5" t="s">
         <v>268</v>
       </c>
-      <c r="F110" s="5" t="s">
+      <c r="E110" s="5" t="s">
         <v>268</v>
       </c>
       <c r="G110" s="5" t="b">
@@ -29854,7 +29855,7 @@
       <c r="D111" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="F111" s="5" t="s">
+      <c r="E111" s="5" t="s">
         <v>270</v>
       </c>
       <c r="G111" s="5" t="b">
@@ -29886,7 +29887,7 @@
       <c r="D112" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="F112" s="5" t="s">
+      <c r="E112" s="5" t="s">
         <v>270</v>
       </c>
       <c r="G112" s="5" t="b">

</xml_diff>